<commit_message>
feat: use XLSX form extras to fill order template cells
</commit_message>
<xml_diff>
--- a/src/templates/ordem-template.xlsx
+++ b/src/templates/ordem-template.xlsx
@@ -11,7 +11,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="c3BpRE2GlLx8piMVFPD+SpFjS4IA9A285r+wA0CjCaw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="PgyDiIvFrQDStl4nGE9ex16roWipp2p3ktIRlOSCRic="/>
     </ext>
   </extLst>
 </workbook>
@@ -163,7 +163,7 @@
     <numFmt numFmtId="167" formatCode="&quot;R$&quot; #,##0.00"/>
     <numFmt numFmtId="168" formatCode="&quot;R$&quot; #,##0.00;[Red]-&quot;R$&quot; #,##0.00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -283,6 +283,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -292,7 +298,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="47">
     <border/>
     <border>
       <left style="medium">
@@ -677,6 +683,9 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -685,11 +694,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
+      <top style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -698,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="118">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -988,72 +995,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="44" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="44" fillId="0" fontId="21" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="28" fillId="0" fontId="21" numFmtId="43" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="32" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="32" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="30" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="30" fillId="0" fontId="21" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf borderId="29" fillId="0" fontId="21" numFmtId="43" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="29" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="32" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="45" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="45" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="46" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="47" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="43" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="43" fillId="0" fontId="21" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf borderId="46" fillId="0" fontId="21" numFmtId="43" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="47" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="47" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="45" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="43" fillId="0" fontId="19" numFmtId="43" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf borderId="46" fillId="0" fontId="22" numFmtId="43" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18671,16 +18638,18 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" ht="33.75" customHeight="1">
+    <row r="25" ht="30.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="114"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="117"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="119"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="116" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="117"/>
       <c r="J25" s="11"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -18699,16 +18668,16 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" ht="51.75" customHeight="1">
+    <row r="26" ht="6.0" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="117"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="119"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="100"/>
       <c r="J26" s="11"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -18727,16 +18696,18 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" ht="32.25" customHeight="1">
+    <row r="27" ht="18.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="117"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="119"/>
+      <c r="C27" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
       <c r="J27" s="11"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -18755,16 +18726,16 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" ht="45.0" customHeight="1">
+    <row r="28" ht="52.5" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="117"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="119"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="18"/>
       <c r="J28" s="11"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -18783,16 +18754,16 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" ht="45.75" customHeight="1">
+    <row r="29" ht="6.0" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="114"/>
-      <c r="D29" s="115"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="117"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="119"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
       <c r="J29" s="11"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -18811,16 +18782,20 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" ht="29.25" customHeight="1">
+    <row r="30" ht="18.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="117"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="119"/>
+      <c r="C30" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="86"/>
+      <c r="E30" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="86"/>
       <c r="J30" s="11"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -18839,16 +18814,16 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" ht="25.5" customHeight="1">
+    <row r="31" ht="103.5" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="115"/>
-      <c r="E31" s="120"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="117"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="119"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="18"/>
       <c r="J31" s="11"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -18867,17 +18842,17 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" ht="28.5" customHeight="1">
+    <row r="32" ht="6.0" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="120"/>
-      <c r="F32" s="116"/>
-      <c r="G32" s="117"/>
-      <c r="H32" s="118"/>
-      <c r="I32" s="119"/>
-      <c r="J32" s="11"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="93"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -18895,17 +18870,17 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" ht="37.5" customHeight="1">
+    <row r="33" ht="18.0" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="114"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="119"/>
-      <c r="J33" s="11"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -18923,23 +18898,23 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" ht="30.75" customHeight="1">
+    <row r="34" ht="18.0" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="117"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="119"/>
-      <c r="J34" s="11"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="98"/>
+      <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -18951,23 +18926,23 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" ht="35.25" customHeight="1">
+    <row r="35" ht="18.0" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="115"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="117"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="119"/>
-      <c r="J35" s="11"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="98"/>
+      <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -18979,17 +18954,17 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" ht="29.25" customHeight="1">
+    <row r="36" ht="18.0" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="116"/>
-      <c r="G36" s="117"/>
-      <c r="H36" s="118"/>
-      <c r="I36" s="119"/>
-      <c r="J36" s="11"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -19007,17 +18982,17 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" ht="36.0" customHeight="1">
+    <row r="37" ht="18.0" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="114"/>
-      <c r="D37" s="115"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="116"/>
-      <c r="G37" s="117"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="119"/>
-      <c r="J37" s="11"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -19035,17 +19010,17 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" ht="44.25" customHeight="1">
+    <row r="38" ht="18.0" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="114"/>
-      <c r="D38" s="115"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="116"/>
-      <c r="G38" s="117"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="119"/>
-      <c r="J38" s="11"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -19063,17 +19038,17 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" ht="51.75" customHeight="1">
+    <row r="39" ht="18.0" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="116"/>
-      <c r="G39" s="117"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="119"/>
-      <c r="J39" s="11"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -19091,17 +19066,17 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" ht="48.75" customHeight="1">
+    <row r="40" ht="18.0" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="122"/>
-      <c r="D40" s="123"/>
-      <c r="E40" s="124"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="126"/>
-      <c r="H40" s="127"/>
-      <c r="I40" s="128"/>
-      <c r="J40" s="11"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -19119,19 +19094,17 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" ht="30.75" customHeight="1">
+    <row r="41" ht="18.0" customHeight="1">
       <c r="A41" s="1"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="122"/>
-      <c r="D41" s="129"/>
-      <c r="E41" s="129"/>
-      <c r="F41" s="129"/>
-      <c r="G41" s="129"/>
-      <c r="H41" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="I41" s="131"/>
-      <c r="J41" s="11"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -19149,17 +19122,17 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" ht="6.0" customHeight="1">
+    <row r="42" ht="18.0" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="100"/>
-      <c r="J42" s="11"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -19177,19 +19150,17 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" ht="18.75" customHeight="1">
+    <row r="43" ht="18.0" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="11"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -19207,17 +19178,17 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" ht="52.5" customHeight="1">
+    <row r="44" ht="18.0" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="84"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="11"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -19235,9 +19206,9 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" ht="6.0" customHeight="1">
+    <row r="45" ht="18.0" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -19245,7 +19216,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="11"/>
+      <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -19263,21 +19234,17 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" ht="18.75" customHeight="1">
+    <row r="46" ht="18.0" customHeight="1">
       <c r="A46" s="1"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="86"/>
-      <c r="E46" s="85" t="s">
-        <v>37</v>
-      </c>
-      <c r="F46" s="87"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="87"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="11"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -19295,17 +19262,17 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" ht="103.5" customHeight="1">
+    <row r="47" ht="18.0" customHeight="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="11"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -19323,17 +19290,17 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" ht="6.0" customHeight="1">
+    <row r="48" ht="18.0" customHeight="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="91"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="92"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-      <c r="I48" s="92"/>
-      <c r="J48" s="93"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -19355,7 +19322,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="94"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -19383,7 +19350,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="95"/>
+      <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -24447,454 +24414,22 @@
       <c r="Y230" s="1"/>
       <c r="Z230" s="1"/>
     </row>
-    <row r="231" ht="18.0" customHeight="1">
-      <c r="A231" s="1"/>
-      <c r="B231" s="1"/>
-      <c r="C231" s="1"/>
-      <c r="D231" s="1"/>
-      <c r="E231" s="1"/>
-      <c r="F231" s="1"/>
-      <c r="G231" s="1"/>
-      <c r="H231" s="1"/>
-      <c r="I231" s="1"/>
-      <c r="J231" s="1"/>
-      <c r="K231" s="1"/>
-      <c r="L231" s="1"/>
-      <c r="M231" s="1"/>
-      <c r="N231" s="1"/>
-      <c r="O231" s="1"/>
-      <c r="P231" s="1"/>
-      <c r="Q231" s="1"/>
-      <c r="R231" s="1"/>
-      <c r="S231" s="1"/>
-      <c r="T231" s="1"/>
-      <c r="U231" s="1"/>
-      <c r="V231" s="1"/>
-      <c r="W231" s="1"/>
-      <c r="X231" s="1"/>
-      <c r="Y231" s="1"/>
-      <c r="Z231" s="1"/>
-    </row>
-    <row r="232" ht="18.0" customHeight="1">
-      <c r="A232" s="1"/>
-      <c r="B232" s="1"/>
-      <c r="C232" s="1"/>
-      <c r="D232" s="1"/>
-      <c r="E232" s="1"/>
-      <c r="F232" s="1"/>
-      <c r="G232" s="1"/>
-      <c r="H232" s="1"/>
-      <c r="I232" s="1"/>
-      <c r="J232" s="1"/>
-      <c r="K232" s="1"/>
-      <c r="L232" s="1"/>
-      <c r="M232" s="1"/>
-      <c r="N232" s="1"/>
-      <c r="O232" s="1"/>
-      <c r="P232" s="1"/>
-      <c r="Q232" s="1"/>
-      <c r="R232" s="1"/>
-      <c r="S232" s="1"/>
-      <c r="T232" s="1"/>
-      <c r="U232" s="1"/>
-      <c r="V232" s="1"/>
-      <c r="W232" s="1"/>
-      <c r="X232" s="1"/>
-      <c r="Y232" s="1"/>
-      <c r="Z232" s="1"/>
-    </row>
-    <row r="233" ht="18.0" customHeight="1">
-      <c r="A233" s="1"/>
-      <c r="B233" s="1"/>
-      <c r="C233" s="1"/>
-      <c r="D233" s="1"/>
-      <c r="E233" s="1"/>
-      <c r="F233" s="1"/>
-      <c r="G233" s="1"/>
-      <c r="H233" s="1"/>
-      <c r="I233" s="1"/>
-      <c r="J233" s="1"/>
-      <c r="K233" s="1"/>
-      <c r="L233" s="1"/>
-      <c r="M233" s="1"/>
-      <c r="N233" s="1"/>
-      <c r="O233" s="1"/>
-      <c r="P233" s="1"/>
-      <c r="Q233" s="1"/>
-      <c r="R233" s="1"/>
-      <c r="S233" s="1"/>
-      <c r="T233" s="1"/>
-      <c r="U233" s="1"/>
-      <c r="V233" s="1"/>
-      <c r="W233" s="1"/>
-      <c r="X233" s="1"/>
-      <c r="Y233" s="1"/>
-      <c r="Z233" s="1"/>
-    </row>
-    <row r="234" ht="18.0" customHeight="1">
-      <c r="A234" s="1"/>
-      <c r="B234" s="1"/>
-      <c r="C234" s="1"/>
-      <c r="D234" s="1"/>
-      <c r="E234" s="1"/>
-      <c r="F234" s="1"/>
-      <c r="G234" s="1"/>
-      <c r="H234" s="1"/>
-      <c r="I234" s="1"/>
-      <c r="J234" s="1"/>
-      <c r="K234" s="1"/>
-      <c r="L234" s="1"/>
-      <c r="M234" s="1"/>
-      <c r="N234" s="1"/>
-      <c r="O234" s="1"/>
-      <c r="P234" s="1"/>
-      <c r="Q234" s="1"/>
-      <c r="R234" s="1"/>
-      <c r="S234" s="1"/>
-      <c r="T234" s="1"/>
-      <c r="U234" s="1"/>
-      <c r="V234" s="1"/>
-      <c r="W234" s="1"/>
-      <c r="X234" s="1"/>
-      <c r="Y234" s="1"/>
-      <c r="Z234" s="1"/>
-    </row>
-    <row r="235" ht="18.0" customHeight="1">
-      <c r="A235" s="1"/>
-      <c r="B235" s="1"/>
-      <c r="C235" s="1"/>
-      <c r="D235" s="1"/>
-      <c r="E235" s="1"/>
-      <c r="F235" s="1"/>
-      <c r="G235" s="1"/>
-      <c r="H235" s="1"/>
-      <c r="I235" s="1"/>
-      <c r="J235" s="1"/>
-      <c r="K235" s="1"/>
-      <c r="L235" s="1"/>
-      <c r="M235" s="1"/>
-      <c r="N235" s="1"/>
-      <c r="O235" s="1"/>
-      <c r="P235" s="1"/>
-      <c r="Q235" s="1"/>
-      <c r="R235" s="1"/>
-      <c r="S235" s="1"/>
-      <c r="T235" s="1"/>
-      <c r="U235" s="1"/>
-      <c r="V235" s="1"/>
-      <c r="W235" s="1"/>
-      <c r="X235" s="1"/>
-      <c r="Y235" s="1"/>
-      <c r="Z235" s="1"/>
-    </row>
-    <row r="236" ht="18.0" customHeight="1">
-      <c r="A236" s="1"/>
-      <c r="B236" s="1"/>
-      <c r="C236" s="1"/>
-      <c r="D236" s="1"/>
-      <c r="E236" s="1"/>
-      <c r="F236" s="1"/>
-      <c r="G236" s="1"/>
-      <c r="H236" s="1"/>
-      <c r="I236" s="1"/>
-      <c r="J236" s="1"/>
-      <c r="K236" s="1"/>
-      <c r="L236" s="1"/>
-      <c r="M236" s="1"/>
-      <c r="N236" s="1"/>
-      <c r="O236" s="1"/>
-      <c r="P236" s="1"/>
-      <c r="Q236" s="1"/>
-      <c r="R236" s="1"/>
-      <c r="S236" s="1"/>
-      <c r="T236" s="1"/>
-      <c r="U236" s="1"/>
-      <c r="V236" s="1"/>
-      <c r="W236" s="1"/>
-      <c r="X236" s="1"/>
-      <c r="Y236" s="1"/>
-      <c r="Z236" s="1"/>
-    </row>
-    <row r="237" ht="18.0" customHeight="1">
-      <c r="A237" s="1"/>
-      <c r="B237" s="1"/>
-      <c r="C237" s="1"/>
-      <c r="D237" s="1"/>
-      <c r="E237" s="1"/>
-      <c r="F237" s="1"/>
-      <c r="G237" s="1"/>
-      <c r="H237" s="1"/>
-      <c r="I237" s="1"/>
-      <c r="J237" s="1"/>
-      <c r="K237" s="1"/>
-      <c r="L237" s="1"/>
-      <c r="M237" s="1"/>
-      <c r="N237" s="1"/>
-      <c r="O237" s="1"/>
-      <c r="P237" s="1"/>
-      <c r="Q237" s="1"/>
-      <c r="R237" s="1"/>
-      <c r="S237" s="1"/>
-      <c r="T237" s="1"/>
-      <c r="U237" s="1"/>
-      <c r="V237" s="1"/>
-      <c r="W237" s="1"/>
-      <c r="X237" s="1"/>
-      <c r="Y237" s="1"/>
-      <c r="Z237" s="1"/>
-    </row>
-    <row r="238" ht="18.0" customHeight="1">
-      <c r="A238" s="1"/>
-      <c r="B238" s="1"/>
-      <c r="C238" s="1"/>
-      <c r="D238" s="1"/>
-      <c r="E238" s="1"/>
-      <c r="F238" s="1"/>
-      <c r="G238" s="1"/>
-      <c r="H238" s="1"/>
-      <c r="I238" s="1"/>
-      <c r="J238" s="1"/>
-      <c r="K238" s="1"/>
-      <c r="L238" s="1"/>
-      <c r="M238" s="1"/>
-      <c r="N238" s="1"/>
-      <c r="O238" s="1"/>
-      <c r="P238" s="1"/>
-      <c r="Q238" s="1"/>
-      <c r="R238" s="1"/>
-      <c r="S238" s="1"/>
-      <c r="T238" s="1"/>
-      <c r="U238" s="1"/>
-      <c r="V238" s="1"/>
-      <c r="W238" s="1"/>
-      <c r="X238" s="1"/>
-      <c r="Y238" s="1"/>
-      <c r="Z238" s="1"/>
-    </row>
-    <row r="239" ht="18.0" customHeight="1">
-      <c r="A239" s="1"/>
-      <c r="B239" s="1"/>
-      <c r="C239" s="1"/>
-      <c r="D239" s="1"/>
-      <c r="E239" s="1"/>
-      <c r="F239" s="1"/>
-      <c r="G239" s="1"/>
-      <c r="H239" s="1"/>
-      <c r="I239" s="1"/>
-      <c r="J239" s="1"/>
-      <c r="K239" s="1"/>
-      <c r="L239" s="1"/>
-      <c r="M239" s="1"/>
-      <c r="N239" s="1"/>
-      <c r="O239" s="1"/>
-      <c r="P239" s="1"/>
-      <c r="Q239" s="1"/>
-      <c r="R239" s="1"/>
-      <c r="S239" s="1"/>
-      <c r="T239" s="1"/>
-      <c r="U239" s="1"/>
-      <c r="V239" s="1"/>
-      <c r="W239" s="1"/>
-      <c r="X239" s="1"/>
-      <c r="Y239" s="1"/>
-      <c r="Z239" s="1"/>
-    </row>
-    <row r="240" ht="18.0" customHeight="1">
-      <c r="A240" s="1"/>
-      <c r="B240" s="1"/>
-      <c r="C240" s="1"/>
-      <c r="D240" s="1"/>
-      <c r="E240" s="1"/>
-      <c r="F240" s="1"/>
-      <c r="G240" s="1"/>
-      <c r="H240" s="1"/>
-      <c r="I240" s="1"/>
-      <c r="J240" s="1"/>
-      <c r="K240" s="1"/>
-      <c r="L240" s="1"/>
-      <c r="M240" s="1"/>
-      <c r="N240" s="1"/>
-      <c r="O240" s="1"/>
-      <c r="P240" s="1"/>
-      <c r="Q240" s="1"/>
-      <c r="R240" s="1"/>
-      <c r="S240" s="1"/>
-      <c r="T240" s="1"/>
-      <c r="U240" s="1"/>
-      <c r="V240" s="1"/>
-      <c r="W240" s="1"/>
-      <c r="X240" s="1"/>
-      <c r="Y240" s="1"/>
-      <c r="Z240" s="1"/>
-    </row>
-    <row r="241" ht="18.0" customHeight="1">
-      <c r="A241" s="1"/>
-      <c r="B241" s="1"/>
-      <c r="C241" s="1"/>
-      <c r="D241" s="1"/>
-      <c r="E241" s="1"/>
-      <c r="F241" s="1"/>
-      <c r="G241" s="1"/>
-      <c r="H241" s="1"/>
-      <c r="I241" s="1"/>
-      <c r="J241" s="1"/>
-      <c r="K241" s="1"/>
-      <c r="L241" s="1"/>
-      <c r="M241" s="1"/>
-      <c r="N241" s="1"/>
-      <c r="O241" s="1"/>
-      <c r="P241" s="1"/>
-      <c r="Q241" s="1"/>
-      <c r="R241" s="1"/>
-      <c r="S241" s="1"/>
-      <c r="T241" s="1"/>
-      <c r="U241" s="1"/>
-      <c r="V241" s="1"/>
-      <c r="W241" s="1"/>
-      <c r="X241" s="1"/>
-      <c r="Y241" s="1"/>
-      <c r="Z241" s="1"/>
-    </row>
-    <row r="242" ht="18.0" customHeight="1">
-      <c r="A242" s="1"/>
-      <c r="B242" s="1"/>
-      <c r="C242" s="1"/>
-      <c r="D242" s="1"/>
-      <c r="E242" s="1"/>
-      <c r="F242" s="1"/>
-      <c r="G242" s="1"/>
-      <c r="H242" s="1"/>
-      <c r="I242" s="1"/>
-      <c r="J242" s="1"/>
-      <c r="K242" s="1"/>
-      <c r="L242" s="1"/>
-      <c r="M242" s="1"/>
-      <c r="N242" s="1"/>
-      <c r="O242" s="1"/>
-      <c r="P242" s="1"/>
-      <c r="Q242" s="1"/>
-      <c r="R242" s="1"/>
-      <c r="S242" s="1"/>
-      <c r="T242" s="1"/>
-      <c r="U242" s="1"/>
-      <c r="V242" s="1"/>
-      <c r="W242" s="1"/>
-      <c r="X242" s="1"/>
-      <c r="Y242" s="1"/>
-      <c r="Z242" s="1"/>
-    </row>
-    <row r="243" ht="18.0" customHeight="1">
-      <c r="A243" s="1"/>
-      <c r="B243" s="1"/>
-      <c r="C243" s="1"/>
-      <c r="D243" s="1"/>
-      <c r="E243" s="1"/>
-      <c r="F243" s="1"/>
-      <c r="G243" s="1"/>
-      <c r="H243" s="1"/>
-      <c r="I243" s="1"/>
-      <c r="J243" s="1"/>
-      <c r="K243" s="1"/>
-      <c r="L243" s="1"/>
-      <c r="M243" s="1"/>
-      <c r="N243" s="1"/>
-      <c r="O243" s="1"/>
-      <c r="P243" s="1"/>
-      <c r="Q243" s="1"/>
-      <c r="R243" s="1"/>
-      <c r="S243" s="1"/>
-      <c r="T243" s="1"/>
-      <c r="U243" s="1"/>
-      <c r="V243" s="1"/>
-      <c r="W243" s="1"/>
-      <c r="X243" s="1"/>
-      <c r="Y243" s="1"/>
-      <c r="Z243" s="1"/>
-    </row>
-    <row r="244" ht="18.0" customHeight="1">
-      <c r="A244" s="1"/>
-      <c r="B244" s="1"/>
-      <c r="C244" s="1"/>
-      <c r="D244" s="1"/>
-      <c r="E244" s="1"/>
-      <c r="F244" s="1"/>
-      <c r="G244" s="1"/>
-      <c r="H244" s="1"/>
-      <c r="I244" s="1"/>
-      <c r="J244" s="1"/>
-      <c r="K244" s="1"/>
-      <c r="L244" s="1"/>
-      <c r="M244" s="1"/>
-      <c r="N244" s="1"/>
-      <c r="O244" s="1"/>
-      <c r="P244" s="1"/>
-      <c r="Q244" s="1"/>
-      <c r="R244" s="1"/>
-      <c r="S244" s="1"/>
-      <c r="T244" s="1"/>
-      <c r="U244" s="1"/>
-      <c r="V244" s="1"/>
-      <c r="W244" s="1"/>
-      <c r="X244" s="1"/>
-      <c r="Y244" s="1"/>
-      <c r="Z244" s="1"/>
-    </row>
-    <row r="245" ht="18.0" customHeight="1">
-      <c r="A245" s="1"/>
-      <c r="B245" s="1"/>
-      <c r="C245" s="1"/>
-      <c r="D245" s="1"/>
-      <c r="E245" s="1"/>
-      <c r="F245" s="1"/>
-      <c r="G245" s="1"/>
-      <c r="H245" s="1"/>
-      <c r="I245" s="1"/>
-      <c r="J245" s="1"/>
-      <c r="K245" s="1"/>
-      <c r="L245" s="1"/>
-      <c r="M245" s="1"/>
-      <c r="N245" s="1"/>
-      <c r="O245" s="1"/>
-      <c r="P245" s="1"/>
-      <c r="Q245" s="1"/>
-      <c r="R245" s="1"/>
-      <c r="S245" s="1"/>
-      <c r="T245" s="1"/>
-      <c r="U245" s="1"/>
-      <c r="V245" s="1"/>
-      <c r="W245" s="1"/>
-      <c r="X245" s="1"/>
-      <c r="Y245" s="1"/>
-      <c r="Z245" s="1"/>
-    </row>
-    <row r="246" ht="18.0" customHeight="1">
-      <c r="A246" s="1"/>
-      <c r="B246" s="1"/>
-      <c r="C246" s="1"/>
-      <c r="D246" s="1"/>
-      <c r="E246" s="1"/>
-      <c r="F246" s="1"/>
-      <c r="G246" s="1"/>
-      <c r="H246" s="1"/>
-      <c r="I246" s="1"/>
-      <c r="J246" s="1"/>
-      <c r="K246" s="1"/>
-      <c r="L246" s="1"/>
-      <c r="M246" s="1"/>
-      <c r="N246" s="1"/>
-      <c r="O246" s="1"/>
-      <c r="P246" s="1"/>
-      <c r="Q246" s="1"/>
-      <c r="R246" s="1"/>
-      <c r="S246" s="1"/>
-      <c r="T246" s="1"/>
-      <c r="U246" s="1"/>
-      <c r="V246" s="1"/>
-      <c r="W246" s="1"/>
-      <c r="X246" s="1"/>
-      <c r="Y246" s="1"/>
-      <c r="Z246" s="1"/>
-    </row>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
     <row r="247" ht="15.75" customHeight="1"/>
     <row r="248" ht="15.75" customHeight="1"/>
     <row r="249" ht="15.75" customHeight="1"/>
@@ -25633,24 +25168,8 @@
     <row r="982" ht="15.75" customHeight="1"/>
     <row r="983" ht="15.75" customHeight="1"/>
     <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="22">
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -25658,6 +25177,14 @@
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="C10:F14"/>
     <mergeCell ref="G16:I16"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:I31"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C20:D21"/>
@@ -25665,26 +25192,6 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C43:I43"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>